<commit_message>
Additional check for Common part
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -271,9 +271,6 @@
     <t>Message_E-1016</t>
   </si>
   <si>
-    <t>Corresponding activity for Incarico verbale autorità not found</t>
-  </si>
-  <si>
     <t>Activity is not Nega Evento or Card non applicable</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>portal.sogesa.net/</t>
+  </si>
+  <si>
+    <t>Corresponding activity '{0}' not found for claim {1}.</t>
   </si>
 </sst>
 </file>
@@ -845,7 +845,7 @@
   <dimension ref="A1:XFD999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9121,13 +9121,13 @@
     </row>
     <row r="6" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2"/>
@@ -17331,125 +17331,125 @@
     </row>
     <row r="8" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384">
       <c r="A11" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="30">
       <c r="A12" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="60">
       <c r="A14" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="14.25" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60">
       <c r="A19" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60">
       <c r="A20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="60">
       <c r="A21" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="60">
       <c r="A22" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -18444,8 +18444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -18711,7 +18711,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -18719,7 +18719,7 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -18727,7 +18727,7 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -18735,7 +18735,7 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -18743,7 +18743,7 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
@@ -18751,7 +18751,7 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
@@ -18759,7 +18759,7 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -18767,7 +18767,7 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -18775,7 +18775,7 @@
         <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
@@ -18783,7 +18783,7 @@
         <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
@@ -18791,7 +18791,7 @@
         <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
@@ -18799,7 +18799,7 @@
         <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -18807,7 +18807,7 @@
         <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
@@ -18815,7 +18815,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
@@ -18823,39 +18823,39 @@
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>